<commit_message>
updated test cases for prospects - TC06, TC07, TC08, TC09
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/NewData.xlsx
+++ b/src/test/resources/TestData/NewData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jteja\GFLAutomation\GFL.Wishes\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9E6A2D-0BA3-4790-BD93-94C9A37994F1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631D04B3-4CE9-49F0-9464-8A06C3FCB838}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="15" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{24025A28-F3F9-43F5-89B1-20F9E5BBA4E0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{24025A28-F3F9-43F5-89B1-20F9E5BBA4E0}"/>
   </bookViews>
   <sheets>
     <sheet name="RunModes" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
interim code update with form validation test cases for sites, prospects
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/NewData.xlsx
+++ b/src/test/resources/TestData/NewData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jteja\GFLAutomation\GFL.Wishes\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37BCF388-8D3C-4D02-BC52-5888FEB1184F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005D8AEF-1C8E-4A05-A3B1-21F36770EA88}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="11" activeTab="18" xr2:uid="{24025A28-F3F9-43F5-89B1-20F9E5BBA4E0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="12600" xr2:uid="{24025A28-F3F9-43F5-89B1-20F9E5BBA4E0}"/>
   </bookViews>
   <sheets>
     <sheet name="RunModes" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="506">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1531,6 +1531,45 @@
   </si>
   <si>
     <t>500</t>
+  </si>
+  <si>
+    <t>SM_NS_FVF_TC01</t>
+  </si>
+  <si>
+    <t>SiteValidation</t>
+  </si>
+  <si>
+    <t>SM_NS_FVF_TC02</t>
+  </si>
+  <si>
+    <t>Site Validation</t>
+  </si>
+  <si>
+    <t>SM_NS_FVF_TC03</t>
+  </si>
+  <si>
+    <t>SM_NS_FVF_TC06</t>
+  </si>
+  <si>
+    <t>SM_NS_FVF_TC05</t>
+  </si>
+  <si>
+    <t>SM_NS_FVF_TC04</t>
+  </si>
+  <si>
+    <t>SM_NS_FVF_TC07</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>zzzzz</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>SM_NS_FVF_TC08</t>
   </si>
 </sst>
 </file>
@@ -1983,10 +2022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA788142-DF31-4F76-877B-06B41CFFA2BE}">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2539,6 +2578,1138 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
     </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="3"/>
+      <c r="L50" s="3"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="3"/>
+      <c r="L53" s="3"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+      <c r="I54" s="3"/>
+      <c r="J54" s="3"/>
+      <c r="K54" s="3"/>
+      <c r="L54" s="3"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+      <c r="L56" s="3"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="3"/>
+      <c r="J57" s="3"/>
+      <c r="K57" s="3"/>
+      <c r="L57" s="3"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
+      <c r="K58" s="3"/>
+      <c r="L58" s="3"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="4"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
+      <c r="J59" s="3"/>
+      <c r="K59" s="3"/>
+      <c r="L59" s="3"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="4"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="3"/>
+      <c r="L60" s="3"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
+      <c r="K61" s="3"/>
+      <c r="L61" s="3"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" s="4"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="3"/>
+      <c r="L62" s="3"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+      <c r="I63" s="3"/>
+      <c r="J63" s="3"/>
+      <c r="K63" s="3"/>
+      <c r="L63" s="3"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="4"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="3"/>
+      <c r="J64" s="3"/>
+      <c r="K64" s="3"/>
+      <c r="L64" s="3"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" s="4"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
+      <c r="J65" s="3"/>
+      <c r="K65" s="3"/>
+      <c r="L65" s="3"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" s="4"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3"/>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="3"/>
+      <c r="L66" s="3"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" s="4"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="3"/>
+      <c r="L67" s="3"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" s="4"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" s="4"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="3"/>
+      <c r="J69" s="3"/>
+      <c r="K69" s="3"/>
+      <c r="L69" s="3"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" s="4"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="3"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="3"/>
+      <c r="L70" s="3"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" s="4"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="3"/>
+      <c r="J71" s="3"/>
+      <c r="K71" s="3"/>
+      <c r="L71" s="3"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" s="4"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3"/>
+      <c r="I72" s="3"/>
+      <c r="J72" s="3"/>
+      <c r="K72" s="3"/>
+      <c r="L72" s="3"/>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" s="4"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+      <c r="J73" s="3"/>
+      <c r="K73" s="3"/>
+      <c r="L73" s="3"/>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" s="4"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="3"/>
+      <c r="L74" s="3"/>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" s="4"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="3"/>
+      <c r="J75" s="3"/>
+      <c r="K75" s="3"/>
+      <c r="L75" s="3"/>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" s="4"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="3"/>
+      <c r="J76" s="3"/>
+      <c r="K76" s="3"/>
+      <c r="L76" s="3"/>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" s="4"/>
+      <c r="B77" s="2"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
+      <c r="H77" s="3"/>
+      <c r="I77" s="3"/>
+      <c r="J77" s="3"/>
+      <c r="K77" s="3"/>
+      <c r="L77" s="3"/>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78" s="4"/>
+      <c r="B78" s="2"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="3"/>
+      <c r="H78" s="3"/>
+      <c r="I78" s="3"/>
+      <c r="J78" s="3"/>
+      <c r="K78" s="3"/>
+      <c r="L78" s="3"/>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A79" s="4"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="3"/>
+      <c r="H79" s="3"/>
+      <c r="I79" s="3"/>
+      <c r="J79" s="3"/>
+      <c r="K79" s="3"/>
+      <c r="L79" s="3"/>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A80" s="4"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="3"/>
+      <c r="H80" s="3"/>
+      <c r="I80" s="3"/>
+      <c r="J80" s="3"/>
+      <c r="K80" s="3"/>
+      <c r="L80" s="3"/>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A81" s="4"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
+      <c r="H81" s="3"/>
+      <c r="I81" s="3"/>
+      <c r="J81" s="3"/>
+      <c r="K81" s="3"/>
+      <c r="L81" s="3"/>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82" s="4"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
+      <c r="H82" s="3"/>
+      <c r="I82" s="3"/>
+      <c r="J82" s="3"/>
+      <c r="K82" s="3"/>
+      <c r="L82" s="3"/>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83" s="4"/>
+      <c r="B83" s="2"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+      <c r="H83" s="3"/>
+      <c r="I83" s="3"/>
+      <c r="J83" s="3"/>
+      <c r="K83" s="3"/>
+      <c r="L83" s="3"/>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84" s="4"/>
+      <c r="B84" s="2"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3"/>
+      <c r="G84" s="3"/>
+      <c r="H84" s="3"/>
+      <c r="I84" s="3"/>
+      <c r="J84" s="3"/>
+      <c r="K84" s="3"/>
+      <c r="L84" s="3"/>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A85" s="4"/>
+      <c r="B85" s="2"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
+      <c r="G85" s="3"/>
+      <c r="H85" s="3"/>
+      <c r="I85" s="3"/>
+      <c r="J85" s="3"/>
+      <c r="K85" s="3"/>
+      <c r="L85" s="3"/>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86" s="4"/>
+      <c r="B86" s="2"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3"/>
+      <c r="G86" s="3"/>
+      <c r="H86" s="3"/>
+      <c r="I86" s="3"/>
+      <c r="J86" s="3"/>
+      <c r="K86" s="3"/>
+      <c r="L86" s="3"/>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87" s="4"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+      <c r="G87" s="3"/>
+      <c r="H87" s="3"/>
+      <c r="I87" s="3"/>
+      <c r="J87" s="3"/>
+      <c r="K87" s="3"/>
+      <c r="L87" s="3"/>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A88" s="4"/>
+      <c r="B88" s="2"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="3"/>
+      <c r="H88" s="3"/>
+      <c r="I88" s="3"/>
+      <c r="J88" s="3"/>
+      <c r="K88" s="3"/>
+      <c r="L88" s="3"/>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A89" s="4"/>
+      <c r="B89" s="2"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3"/>
+      <c r="G89" s="3"/>
+      <c r="H89" s="3"/>
+      <c r="I89" s="3"/>
+      <c r="J89" s="3"/>
+      <c r="K89" s="3"/>
+      <c r="L89" s="3"/>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A90" s="4"/>
+      <c r="B90" s="2"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
+      <c r="G90" s="3"/>
+      <c r="H90" s="3"/>
+      <c r="I90" s="3"/>
+      <c r="J90" s="3"/>
+      <c r="K90" s="3"/>
+      <c r="L90" s="3"/>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A91" s="4"/>
+      <c r="B91" s="2"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
+      <c r="H91" s="3"/>
+      <c r="I91" s="3"/>
+      <c r="J91" s="3"/>
+      <c r="K91" s="3"/>
+      <c r="L91" s="3"/>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A92" s="4"/>
+      <c r="B92" s="2"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3"/>
+      <c r="G92" s="3"/>
+      <c r="H92" s="3"/>
+      <c r="I92" s="3"/>
+      <c r="J92" s="3"/>
+      <c r="K92" s="3"/>
+      <c r="L92" s="3"/>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A93" s="4"/>
+      <c r="B93" s="2"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="3"/>
+      <c r="G93" s="3"/>
+      <c r="H93" s="3"/>
+      <c r="I93" s="3"/>
+      <c r="J93" s="3"/>
+      <c r="K93" s="3"/>
+      <c r="L93" s="3"/>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A94" s="4"/>
+      <c r="B94" s="2"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="3"/>
+      <c r="G94" s="3"/>
+      <c r="H94" s="3"/>
+      <c r="I94" s="3"/>
+      <c r="J94" s="3"/>
+      <c r="K94" s="3"/>
+      <c r="L94" s="3"/>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A95" s="4"/>
+      <c r="B95" s="2"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="3"/>
+      <c r="G95" s="3"/>
+      <c r="H95" s="3"/>
+      <c r="I95" s="3"/>
+      <c r="J95" s="3"/>
+      <c r="K95" s="3"/>
+      <c r="L95" s="3"/>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A96" s="4"/>
+      <c r="B96" s="2"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="3"/>
+      <c r="G96" s="3"/>
+      <c r="H96" s="3"/>
+      <c r="I96" s="3"/>
+      <c r="J96" s="3"/>
+      <c r="K96" s="3"/>
+      <c r="L96" s="3"/>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A97" s="4"/>
+      <c r="B97" s="2"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="3"/>
+      <c r="G97" s="3"/>
+      <c r="H97" s="3"/>
+      <c r="I97" s="3"/>
+      <c r="J97" s="3"/>
+      <c r="K97" s="3"/>
+      <c r="L97" s="3"/>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A98" s="4"/>
+      <c r="B98" s="2"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="3"/>
+      <c r="G98" s="3"/>
+      <c r="H98" s="3"/>
+      <c r="I98" s="3"/>
+      <c r="J98" s="3"/>
+      <c r="K98" s="3"/>
+      <c r="L98" s="3"/>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A99" s="4"/>
+      <c r="B99" s="2"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="3"/>
+      <c r="G99" s="3"/>
+      <c r="H99" s="3"/>
+      <c r="I99" s="3"/>
+      <c r="J99" s="3"/>
+      <c r="K99" s="3"/>
+      <c r="L99" s="3"/>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A100" s="4"/>
+      <c r="B100" s="2"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3"/>
+      <c r="G100" s="3"/>
+      <c r="H100" s="3"/>
+      <c r="I100" s="3"/>
+      <c r="J100" s="3"/>
+      <c r="K100" s="3"/>
+      <c r="L100" s="3"/>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A101" s="4"/>
+      <c r="B101" s="2"/>
+      <c r="C101" s="3"/>
+      <c r="D101" s="3"/>
+      <c r="E101" s="3"/>
+      <c r="F101" s="3"/>
+      <c r="G101" s="3"/>
+      <c r="H101" s="3"/>
+      <c r="I101" s="3"/>
+      <c r="J101" s="3"/>
+      <c r="K101" s="3"/>
+      <c r="L101" s="3"/>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A102" s="4"/>
+      <c r="B102" s="2"/>
+      <c r="C102" s="3"/>
+      <c r="D102" s="3"/>
+      <c r="E102" s="3"/>
+      <c r="F102" s="3"/>
+      <c r="G102" s="3"/>
+      <c r="H102" s="3"/>
+      <c r="I102" s="3"/>
+      <c r="J102" s="3"/>
+      <c r="K102" s="3"/>
+      <c r="L102" s="3"/>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A103" s="4"/>
+      <c r="B103" s="2"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
+      <c r="E103" s="3"/>
+      <c r="F103" s="3"/>
+      <c r="G103" s="3"/>
+      <c r="H103" s="3"/>
+      <c r="I103" s="3"/>
+      <c r="J103" s="3"/>
+      <c r="K103" s="3"/>
+      <c r="L103" s="3"/>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A104" s="4"/>
+      <c r="B104" s="2"/>
+      <c r="C104" s="3"/>
+      <c r="D104" s="3"/>
+      <c r="E104" s="3"/>
+      <c r="F104" s="3"/>
+      <c r="G104" s="3"/>
+      <c r="H104" s="3"/>
+      <c r="I104" s="3"/>
+      <c r="J104" s="3"/>
+      <c r="K104" s="3"/>
+      <c r="L104" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:L1"/>
@@ -2547,7 +3718,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N17:N20" xr:uid="{B4FD6766-A32F-44AA-8CFB-2BD8E71B2F82}">
       <formula1>$A$2:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:L27" xr:uid="{27706EAA-48C0-4360-826C-27E4471783EC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:L27 C28:G28 C29:E29 C30:D30 C31:L104" xr:uid="{27706EAA-48C0-4360-826C-27E4471783EC}">
       <formula1>$A$2:$A$50</formula1>
     </dataValidation>
   </dataValidations>
@@ -2585,22 +3756,24 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51DAE5B4-B963-47A4-B2A4-C45BD479A193}">
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" style="8" customWidth="1"/>
     <col min="2" max="2" width="41" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="22.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="11" width="23.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="8"/>
+    <col min="3" max="4" width="22.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="23.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>52</v>
       </c>
@@ -2613,39 +3786,47 @@
       <c r="D1" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="8" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>247</v>
       </c>
@@ -2655,46 +3836,56 @@
       <c r="D8" s="8" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="8" t="s">
+        <v>504</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="8" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>255</v>
       </c>
+      <c r="E16" s="12"/>
     </row>
     <row r="17" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
@@ -2827,6 +4018,7 @@
     <row r="57" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3005,21 +4197,23 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{417BFBCF-E3E0-4816-AF93-8ADED1A6AB9A}">
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" style="8" customWidth="1"/>
     <col min="2" max="2" width="39.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="22.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="8"/>
+    <col min="3" max="7" width="22.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" style="8" customWidth="1"/>
+    <col min="9" max="10" width="22.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>52</v>
       </c>
@@ -3032,13 +4226,24 @@
       <c r="D1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="J1" s="7"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
         <v>289</v>
       </c>
@@ -3048,8 +4253,23 @@
       <c r="D2" s="8" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="8" t="s">
+        <v>494</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>494</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>496</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>496</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>290</v>
       </c>
@@ -3060,7 +4280,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>291</v>
       </c>
@@ -3071,7 +4291,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>292</v>
       </c>
@@ -3082,7 +4302,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>293</v>
       </c>
@@ -3093,7 +4313,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>294</v>
       </c>
@@ -3104,7 +4324,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>295</v>
       </c>
@@ -3115,7 +4335,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>296</v>
       </c>
@@ -3126,7 +4346,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>297</v>
       </c>
@@ -3137,7 +4357,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>298</v>
       </c>
@@ -3148,7 +4368,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>299</v>
       </c>
@@ -3159,7 +4379,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>300</v>
       </c>
@@ -3171,7 +4391,7 @@
       </c>
       <c r="E13" s="10"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
         <v>301</v>
       </c>
@@ -3182,7 +4402,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>302</v>
       </c>
@@ -3193,7 +4413,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>303</v>
       </c>
@@ -3514,8 +4734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D89BA3D3-1B94-4C77-B8E7-B6D246A7B5C9}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4283,13 +5503,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8524A69F-58DC-4C12-B71C-F15E36FF1DB4}">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="19" topLeftCell="D20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="19" topLeftCell="J30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="L1" sqref="L1"/>
+      <selection pane="bottomRight" activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4298,10 +5518,11 @@
     <col min="2" max="2" width="38" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="11" width="21.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="7.7109375" style="8"/>
+    <col min="13" max="16" width="16.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="7.7109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>52</v>
       </c>
@@ -4338,13 +5559,25 @@
       <c r="L1" s="2" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>55</v>
       </c>
@@ -4375,8 +5608,14 @@
       <c r="L3" s="8" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="M3" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>57</v>
       </c>
@@ -4407,75 +5646,105 @@
       <c r="L4" s="8" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="8" t="s">
+        <v>493</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>63</v>
       </c>
       <c r="K10" s="8" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N10" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="P10" s="8" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>64</v>
       </c>
       <c r="K11" s="8" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="N11" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="P11" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>65</v>
       </c>
       <c r="K12" s="8" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N12" s="8" t="s">
+        <v>493</v>
+      </c>
+      <c r="P12" s="8" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>66</v>
       </c>
       <c r="K13" s="8" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N13" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="P13" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>69</v>
       </c>
@@ -4560,12 +5829,18 @@
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
         <v>86</v>
       </c>
       <c r="K33" s="8" t="s">
         <v>466</v>
+      </c>
+      <c r="N33" s="8" t="s">
+        <v>493</v>
+      </c>
+      <c r="P33" s="8" t="s">
+        <v>493</v>
       </c>
     </row>
   </sheetData>
@@ -4576,14 +5851,14 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBCAE703-B904-44CB-A990-CED3724569EE}">
-  <dimension ref="A1:J56"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="18" topLeftCell="C31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="18" topLeftCell="G19" activePane="bottomRight" state="frozen"/>
       <selection activeCell="G19" sqref="G19"/>
       <selection pane="topRight" activeCell="G19" sqref="G19"/>
       <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
-      <selection pane="bottomRight" activeCell="J48" sqref="J48"/>
+      <selection pane="bottomRight" activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4592,10 +5867,12 @@
     <col min="2" max="2" width="46" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="21.5703125" style="8" customWidth="1"/>
     <col min="6" max="9" width="21.42578125" style="8" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="8"/>
+    <col min="10" max="10" width="9.140625" style="8"/>
+    <col min="11" max="11" width="16.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>52</v>
       </c>
@@ -4626,8 +5903,11 @@
       <c r="J1" s="2" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
         <v>87</v>
       </c>
@@ -4655,8 +5935,11 @@
       <c r="J2" s="8" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K2" s="8" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>88</v>
       </c>
@@ -4668,7 +5951,7 @@
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>89</v>
       </c>
@@ -4693,8 +5976,11 @@
       <c r="J4" s="8" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>91</v>
       </c>
@@ -4722,8 +6008,11 @@
       <c r="J5" s="8" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="8" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>92</v>
       </c>
@@ -4751,48 +6040,51 @@
       <c r="J6" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>102</v>
       </c>
@@ -4809,7 +6101,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>103</v>
       </c>
@@ -5507,7 +6799,7 @@
   <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1048576"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>